<commit_message>
getting the differeces of annotations
</commit_message>
<xml_diff>
--- a/notebooks_rotten_tomatoes_static_lex/test_cases/approach5.xlsx
+++ b/notebooks_rotten_tomatoes_static_lex/test_cases/approach5.xlsx
@@ -1095,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,7 +1128,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>less cinematically wonderful than quietly and deeply moving , which is wonderful in itself .</t>
+          <t>less cinematically worth than quietly and deeply moving , which is worth in itself .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1146,7 +1146,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>less cinematically powerful than quietly and deeply moving , which is powerful in itself .</t>
+          <t>less cinematically imitative than quietly and deeply moving , which is imitative in itself .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1164,7 +1164,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>less cinematically imitative than quietly and deeply moving , which is imitative in itself .</t>
+          <t>less cinematically wonderful than quietly and deeply moving , which is wonderful in itself .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1182,7 +1182,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>less cinematically worth than quietly and deeply moving , which is worth in itself .</t>
+          <t>less cinematically brilliant than quietly and deeply moving , which is brilliant in itself .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1190,28 +1190,10 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>less cinematically timeless than quietly and deeply moving , which is timeless in itself .</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1226,7 +1208,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1259,7 +1241,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the imitative spectacle of people really combines to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the phenomenal spectacle of people really combines to each other .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1277,7 +1259,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the brilliant spectacle of people really gets to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the phenomenal spectacle of people really carries to each other .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1295,7 +1277,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the funny spectacle of people really gets to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the passionate spectacle of people really celebrating to each other .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1313,7 +1295,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the timeless spectacle of people really gets to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the successful spectacle of people really combines to each other .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1331,7 +1313,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the notch spectacle of people really manages to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the engrossing spectacle of people really evoked to each other .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1349,7 +1331,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>pratfalls aside , barbershop gets its greatest play from the wonderful spectacle of people really talking to each other .</t>
+          <t>pratfalls aside , barbershop gets its greatest play from the timeless spectacle of people really shares to each other .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1361,6 +1343,96 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pratfalls aside , barbershop gets its greatest play from the phenomenal spectacle of people really celebrating to each other .</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>pratfalls aside , barbershop gets its greatest play from the successful spectacle of people really celebrating to each other .</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pratfalls aside , barbershop gets its greatest play from the phenomenal spectacle of people really gets to each other .</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>pratfalls aside , barbershop gets its greatest play from the passionate spectacle of people really manages to each other .</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>pratfalls aside , barbershop gets its greatest play from the notch spectacle of people really shares to each other .</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1375,7 +1447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1408,7 +1480,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>an imitative story that combines psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an phenomenal story that combines psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1426,7 +1498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>an brilliant story that gets psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an phenomenal story that carries psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1444,7 +1516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>an funny story that gets psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an passionate story that celebrating psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1462,7 +1534,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>an timeless story that gets psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an successful story that combines psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1480,7 +1552,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>an notch story that manages psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an engrossing story that evoked psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1498,7 +1570,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>an wonderful story that talking psychological drama , sociological reflection , and high - octane thriller .</t>
+          <t>an timeless story that shares psychological drama , sociological reflection , and high - octane thriller .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1510,6 +1582,96 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>an phenomenal story that celebrating psychological drama , sociological reflection , and high - octane thriller .</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>an successful story that celebrating psychological drama , sociological reflection , and high - octane thriller .</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>an phenomenal story that gets psychological drama , sociological reflection , and high - octane thriller .</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>an passionate story that manages psychological drama , sociological reflection , and high - octane thriller .</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>an notch story that shares psychological drama , sociological reflection , and high - octane thriller .</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1524,7 +1686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1557,7 +1719,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>in imax in entire , it 's just as imitative on the big screen .</t>
+          <t>in imax in bad , it 's just as unconditional on the big screen .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1575,7 +1737,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>in imax in expectant , it 's just as imitative on the big screen .</t>
+          <t>in imax in unpretentious , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1593,7 +1755,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>in imax in unpretentious , it 's just as notch on the big screen .</t>
+          <t>in imax in big , it 's just as imitative on the big screen .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1611,7 +1773,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>in imax in sensitive , it 's just as imitative on the big screen .</t>
+          <t>in imax in tiresome , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1629,7 +1791,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>in imax in dumb , it 's just as notch on the big screen .</t>
+          <t>in imax in short , it 's just as imitative on the big screen .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1647,7 +1809,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>in imax in harmless , it 's just as tender on the big screen .</t>
+          <t>in imax in dumb , it 's just as unconditional on the big screen .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1665,7 +1827,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>in imax in manipulative , it 's just as notch on the big screen .</t>
+          <t>in imax in previous , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1683,7 +1845,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>in imax in tiresome , it 's just as notch on the big screen .</t>
+          <t>in imax in dumb , it 's just as tender on the big screen .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1701,7 +1863,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>in imax in unpretentious , it 's just as tender on the big screen .</t>
+          <t>in imax in undeterminable , it 's just as tender on the big screen .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1719,7 +1881,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>in imax in drunk , it 's just as imitative on the big screen .</t>
+          <t>in imax in undeterminable , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1737,7 +1899,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>in imax in tiresome , it 's just as tender on the big screen .</t>
+          <t>in imax in expectant , it 's just as tender on the big screen .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1755,7 +1917,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>in imax in short , it 's just as imitative on the big screen .</t>
+          <t>in imax in stupid , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1773,7 +1935,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>in imax in preposterous , it 's just as tender on the big screen .</t>
+          <t>in imax in nasty , it 's just as imitative on the big screen .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1791,7 +1953,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>in imax in previous , it 's just as notch on the big screen .</t>
+          <t>in imax in manipulative , it 's just as notch on the big screen .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1809,7 +1971,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>in imax in unpretentious , it 's just as imitative on the big screen .</t>
+          <t>in imax in cumbersome , it 's just as imitative on the big screen .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1827,7 +1989,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>in imax in harmless , it 's just as unconditional on the big screen .</t>
+          <t>in imax in preposterous , it 's just as timeless on the big screen .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1845,7 +2007,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>in imax in entire , it 's just as wonderful on the big screen .</t>
+          <t>in imax in short , it 's just as engrossing on the big screen .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1863,7 +2025,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>in imax in wannabe , it 's just as successful on the big screen .</t>
+          <t>in imax in tiresome , it 's just as passionate on the big screen .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1881,7 +2043,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>in imax in unpretentious , it 's just as terrific on the big screen .</t>
+          <t>in imax in big , it 's just as terrific on the big screen .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1899,7 +2061,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>in imax in previous , it 's just as engrossing on the big screen .</t>
+          <t>in imax in stupid , it 's just as successful on the big screen .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1917,7 +2079,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>in imax in short , it 's just as powerful on the big screen .</t>
+          <t>in imax in entire , it 's just as wonderful on the big screen .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1935,7 +2097,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>in imax in dumb , it 's just as timeless on the big screen .</t>
+          <t>in imax in psychopathic , it 's just as powerful on the big screen .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1953,7 +2115,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>in imax in tiresome , it 's just as wonderful on the big screen .</t>
+          <t>in imax in entire , it 's just as worth on the big screen .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1971,7 +2133,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>in imax in cumbersome , it 's just as brilliant on the big screen .</t>
+          <t>in imax in previous , it 's just as powerful on the big screen .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1989,7 +2151,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>in imax in expectant , it 's just as terrific on the big screen .</t>
+          <t>in imax in expectant , it 's just as engrossing on the big screen .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2007,7 +2169,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>in imax in short , it 's just as worth on the big screen .</t>
+          <t>in imax in dumb , it 's just as powerful on the big screen .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -2025,7 +2187,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>in imax in original , it 's just as wonderful on the big screen .</t>
+          <t>in imax in short , it 's just as successful on the big screen .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -2043,7 +2205,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>in imax in psychopathic , it 's just as terrific on the big screen .</t>
+          <t>in imax in entire , it 's just as breathtaking on the big screen .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -2061,7 +2223,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>in imax in drunk , it 's just as phenomenal on the big screen .</t>
+          <t>in imax in off , it 's just as worth on the big screen .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -2079,7 +2241,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>in imax in original , it 's just as brilliant on the big screen .</t>
+          <t>in imax in tiresome , it 's just as timeless on the big screen .</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -2097,7 +2259,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>in imax in original , it 's just as engrossing on the big screen .</t>
+          <t>in imax in psychopathic , it 's just as terrific on the big screen .</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -2115,7 +2277,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>in imax in sensitive , it 's just as powerful on the big screen .</t>
+          <t>in imax in drunk , it 's just as funny on the big screen .</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -2133,7 +2295,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>in imax in harmless , it 's just as brilliant on the big screen .</t>
+          <t>in imax in cumbersome , it 's just as successful on the big screen .</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2151,7 +2313,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>in imax in original , it 's just as powerful on the big screen .</t>
+          <t>in imax in nasty , it 's just as brilliant on the big screen .</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2163,24 +2325,6 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>in imax in psychopathic , it 's just as successful on the big screen .</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2195,7 +2339,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2228,7 +2372,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>the rules of attraction combines us too big on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction enjoy us too unpretentious on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2246,7 +2390,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>the rules of attraction manages us too unpretentious on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction enjoy us too stupid on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2264,7 +2408,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>the rules of attraction talking us too previous on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction evoked us too cumbersome on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2282,7 +2426,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>the rules of attraction combines us too entire on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction carries us too sensitive on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2300,7 +2444,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>the rules of attraction gets us too stupid on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction gets us too drunk on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2318,7 +2462,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>the rules of attraction manages us too stupid on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction combines us too cumbersome on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2336,7 +2480,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>the rules of attraction gets us too psychopathic on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction loved us too off on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2354,7 +2498,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>the rules of attraction gets us too sensitive on the party favors to sober us up with the transparent attempts at moralizing .</t>
+          <t>the rules of attraction shares us too tiresome on the party favors to sober us up with the transparent attempts at moralizing .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2366,6 +2510,132 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>the rules of attraction talking us too entire on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>the rules of attraction enjoy us too original on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>the rules of attraction evoked us too manipulative on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>the rules of attraction celebrating us too dumb on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>the rules of attraction carries us too bad on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>the rules of attraction gets us too entire on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>the rules of attraction talking us too big on the party favors to sober us up with the transparent attempts at moralizing .</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2380,7 +2650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,7 +2683,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>combines to accomplish what few sequels can -- it equals the big and in some ways even betters it .</t>
+          <t>enjoy to accomplish what few sequels can -- it equals the unpretentious and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2431,7 +2701,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>manages to accomplish what few sequels can -- it equals the unpretentious and in some ways even betters it .</t>
+          <t>enjoy to accomplish what few sequels can -- it equals the stupid and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2449,7 +2719,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>talking to accomplish what few sequels can -- it equals the previous and in some ways even betters it .</t>
+          <t>evoked to accomplish what few sequels can -- it equals the cumbersome and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2467,7 +2737,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>combines to accomplish what few sequels can -- it equals the entire and in some ways even betters it .</t>
+          <t>carries to accomplish what few sequels can -- it equals the sensitive and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2485,7 +2755,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>gets to accomplish what few sequels can -- it equals the stupid and in some ways even betters it .</t>
+          <t>gets to accomplish what few sequels can -- it equals the drunk and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2503,7 +2773,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>manages to accomplish what few sequels can -- it equals the stupid and in some ways even betters it .</t>
+          <t>combines to accomplish what few sequels can -- it equals the cumbersome and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2521,7 +2791,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gets to accomplish what few sequels can -- it equals the psychopathic and in some ways even betters it .</t>
+          <t>loved to accomplish what few sequels can -- it equals the off and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2539,7 +2809,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>gets to accomplish what few sequels can -- it equals the sensitive and in some ways even betters it .</t>
+          <t>shares to accomplish what few sequels can -- it equals the tiresome and in some ways even betters it .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2551,6 +2821,132 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>talking to accomplish what few sequels can -- it equals the entire and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>enjoy to accomplish what few sequels can -- it equals the original and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>evoked to accomplish what few sequels can -- it equals the manipulative and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>celebrating to accomplish what few sequels can -- it equals the dumb and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>carries to accomplish what few sequels can -- it equals the bad and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>gets to accomplish what few sequels can -- it equals the entire and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>talking to accomplish what few sequels can -- it equals the big and in some ways even betters it .</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2617,8 +3013,8 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>" one look at a girl in tight pants and big tits and you turn entire ? " um -  . . is n't that the basis for the entire plot ?</t>
+          <t>" one look at a girl in tight pants and big tits and you turn unpretentious ? " um +  . . is n't that the basis for the unpretentious plot ?</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2636,8 +3032,8 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>" one look at a girl in tight pants and big tits and you turn previous ? " um -  . . is n't that the basis for the previous plot ?</t>
+          <t>" one look at a girl in tight pants and big tits and you turn psychopathic ? " um +  . . is n't that the basis for the psychopathic plot ?</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2663,7 +3059,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2696,7 +3092,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally sensitive and sadly worth of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally big and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2714,7 +3110,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally big and sadly tender of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally original and sadly funny of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2732,7 +3128,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally expectant and sadly powerful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally previous and sadly breathtaking of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2750,7 +3146,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally big and sadly unconditional of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally entire and sadly powerful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2768,7 +3164,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally original and sadly notch of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally entire and sadly breathtaking of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2786,7 +3182,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally sensitive and sadly successful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally undeterminable and sadly wonderful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2804,7 +3200,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally short and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2822,7 +3218,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally original and sadly powerful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally original and sadly successful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2840,7 +3236,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally original and sadly wonderful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally wannabe and sadly powerful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2858,7 +3254,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally entire and sadly terrific of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally entire and sadly tender of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2876,7 +3272,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally big and sadly engrossing of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally short and sadly tender of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2894,7 +3290,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally undeterminable and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally original and sadly imitative of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -2912,7 +3308,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally big and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally manipulative and sadly successful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2930,7 +3326,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally entire and sadly powerful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally wannabe and sadly passionate of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2948,7 +3344,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally preposterous and sadly wonderful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally nasty and sadly funny of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -2966,7 +3362,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally expectant and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally sensitive and sadly notch of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2984,7 +3380,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally original and sadly engrossing of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally undeterminable and sadly funny of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -3002,7 +3398,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally previous and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally big and sadly funny of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -3020,7 +3416,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally preposterous and sadly funny of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally original and sadly brilliant of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -3038,7 +3434,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally short and sadly funny of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally entire and sadly unconditional of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -3056,7 +3452,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally wannabe and sadly funny of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally preposterous and sadly passionate of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -3074,7 +3470,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally entire and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally entire and sadly engrossing of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -3092,7 +3488,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally psychopathic and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally short and sadly breathtaking of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -3110,7 +3506,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally entire and sadly unconditional of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally off and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -3128,7 +3524,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally unpretentious and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally tiresome and sadly wonderful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -3146,7 +3542,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally psychopathic and sadly powerful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally original and sadly engrossing of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -3164,7 +3560,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally manipulative and sadly engrossing of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally undeterminable and sadly unconditional of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -3182,7 +3578,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally cumbersome and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally unpretentious and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3200,7 +3596,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly wonderful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally manipulative and sadly breathtaking of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -3218,7 +3614,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally previous and sadly funny of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally manipulative and sadly powerful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -3236,7 +3632,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally manipulative and sadly powerful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally big and sadly brilliant of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -3254,7 +3650,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally expectant and sadly funny of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally expectant and sadly unconditional of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -3272,7 +3668,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally drunk and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally big and sadly engrossing of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -3290,7 +3686,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally sensitive and sadly imitative of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally dumb and sadly breathtaking of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3308,7 +3704,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally short and sadly tender of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally expectant and sadly successful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3326,7 +3722,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly engrossing of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally previous and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3334,17 +3730,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally expectant and sadly notch of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally undeterminable and sadly passionate of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3352,17 +3748,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally harmless and sadly brilliant of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally cumbersome and sadly successful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3370,17 +3766,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly timeless of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally bad and sadly imitative of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -3398,7 +3794,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally stupid and sadly wonderful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally bad and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -3416,7 +3812,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally stupid and sadly engrossing of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally drunk and sadly worth of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -3434,7 +3830,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly tender of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally nasty and sadly timeless of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -3452,7 +3848,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally dumb and sadly worth of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally psychopathic and sadly imitative of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -3470,7 +3866,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally preposterous and sadly phenomenal of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally manipulative and sadly terrific of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -3488,7 +3884,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally tiresome and sadly unconditional of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally drunk and sadly terrific of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -3506,7 +3902,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally short and sadly worth of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally dumb and sadly successful of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -3524,7 +3920,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally stupid and sadly unconditional of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally undeterminable and sadly phenomenal of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -3542,7 +3938,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>charly comes off as emotionally drunk and sadly successful of innumerable past love story derisions .</t>
+          <t>charly comes off as emotionally bad and sadly brilliant of innumerable past love story derisions .</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3554,6 +3950,42 @@
         </is>
       </c>
       <c r="D49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>charly comes off as emotionally tiresome and sadly notch of innumerable past love story derisions .</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>charly comes off as emotionally harmless and sadly terrific of innumerable past love story derisions .</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3601,7 +4033,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tully is imitative a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is imitative a look for its true - to - life characters , its stupid acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -3619,7 +4051,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>tully is imitative a look for its true - to - life characters , its harmless acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is tender a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -3637,7 +4069,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>tully is notch a look for its true - to - life characters , its stupid acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is imitative a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3655,7 +4087,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>tully is imitative a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is tender a look for its true - to - life characters , its bad acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3673,7 +4105,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tully is timeless a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is timeless a look for its true - to - life characters , its bad acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -3691,7 +4123,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>tully is unconditional a look for its true - to - life characters , its big acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is timeless a look for its true - to - life characters , its stupid acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3699,17 +4131,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>tully is imitative a look for its true - to - life characters , its wannabe acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is imitative a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3717,17 +4149,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>tully is worth a look for its true - to - life characters , its cumbersome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is powerful a look for its true - to - life characters , its stupid acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3745,7 +4177,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>tully is engrossing a look for its true - to - life characters , its preposterous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is brilliant a look for its true - to - life characters , its bad acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -3763,7 +4195,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>tully is phenomenal a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is engrossing a look for its true - to - life characters , its off acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -3781,7 +4213,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>tully is worth a look for its true - to - life characters , its preposterous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is wonderful a look for its true - to - life characters , its entire acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -3799,7 +4231,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>tully is powerful a look for its true - to - life characters , its manipulative acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is successful a look for its true - to - life characters , its short acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -3817,7 +4249,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>tully is successful a look for its true - to - life characters , its expectant acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is brilliant a look for its true - to - life characters , its big acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -3835,7 +4267,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>tully is imitative a look for its true - to - life characters , its sensitive acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is breathtaking a look for its true - to - life characters , its nasty acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -3853,7 +4285,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>tully is terrific a look for its true - to - life characters , its preposterous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is powerful a look for its true - to - life characters , its big acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -3871,7 +4303,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>tully is terrific a look for its true - to - life characters , its short acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is worth a look for its true - to - life characters , its harmless acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -3889,7 +4321,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>tully is wonderful a look for its true - to - life characters , its manipulative acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is terrific a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -3907,7 +4339,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>tully is terrific a look for its true - to - life characters , its cumbersome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is engrossing a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -3925,7 +4357,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>tully is worth a look for its true - to - life characters , its big acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is unconditional a look for its true - to - life characters , its nasty acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -3943,7 +4375,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>tully is notch a look for its true - to - life characters , its entire acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is passionate a look for its true - to - life characters , its preposterous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -3961,7 +4393,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>tully is wonderful a look for its true - to - life characters , its sensitive acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is unconditional a look for its true - to - life characters , its expectant acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -3979,7 +4411,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>tully is wonderful a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is engrossing a look for its true - to - life characters , its expectant acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -3997,7 +4429,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>tully is brilliant a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is imitative a look for its true - to - life characters , its cumbersome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -4015,7 +4447,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>tully is worth a look for its true - to - life characters , its tiresome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is brilliant a look for its true - to - life characters , its dumb acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -4033,7 +4465,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>tully is brilliant a look for its true - to - life characters , its stupid acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is unconditional a look for its true - to - life characters , its unpretentious acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -4051,7 +4483,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>tully is tender a look for its true - to - life characters , its previous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is notch a look for its true - to - life characters , its sensitive acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -4069,7 +4501,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>tully is brilliant a look for its true - to - life characters , its preposterous acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is wonderful a look for its true - to - life characters , its cumbersome acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -4087,7 +4519,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>tully is successful a look for its true - to - life characters , its sensitive acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is phenomenal a look for its true - to - life characters , its harmless acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -4105,7 +4537,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>tully is notch a look for its true - to - life characters , its big acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
+          <t>tully is timeless a look for its true - to - life characters , its undeterminable acting , its unadorned view of rural life and the subtle direction of first - timer hilary birmingham .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -4131,7 +4563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4164,7 +4596,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves manipulative , the acting is robotically italicized , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves preposterous , the acting is robotically removed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4182,7 +4614,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves cumbersome , the acting is robotically italicized , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves expectant , the acting is robotically dismissed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4200,7 +4632,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves psychopathic , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves wannabe , the acting is robotically squanders , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4218,7 +4650,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves unpretentious , the acting is robotically dismissed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves tiresome , the acting is robotically withered , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4236,7 +4668,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves preposterous , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves previous , the acting is robotically modeled , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -4254,7 +4686,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves original , the acting is robotically removed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves big , the acting is robotically withered , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -4272,7 +4704,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves cumbersome , the acting is robotically removed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves bad , the acting is robotically avoids , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -4290,7 +4722,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves psychopathic , the acting is robotically removed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves off , the acting is robotically squanders , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4308,7 +4740,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves unpretentious , the acting is robotically modeled , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves entire , the acting is robotically dismissed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4326,7 +4758,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves tiresome , the acting is robotically squanders , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves harmless , the acting is robotically italicized , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4344,7 +4776,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves dumb , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves big , the acting is robotically sum , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -4362,7 +4794,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves entire , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves original , the acting is robotically withered , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -4380,7 +4812,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves harmless , the acting is robotically removed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves expectant , the acting is robotically modeled , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -4398,7 +4830,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves drunk , the acting is robotically avoids , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves stupid , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -4416,7 +4848,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves cumbersome , the acting is robotically sum , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves stupid , the acting is robotically spare , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -4434,7 +4866,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves preposterous , the acting is robotically squanders , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves short , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -4452,7 +4884,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>the high - concept scenario soon proves cumbersome , the acting is robotically simpering , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
+          <t>the high - concept scenario soon proves tiresome , the acting is robotically modeled , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -4464,24 +4896,6 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>the high - concept scenario soon proves cumbersome , the acting is robotically dismissed , and truth - in - advertising hounds take note : there 's very little hustling on view .</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4496,7 +4910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4529,7 +4943,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>manipulative , charming , quirky , manipulative</t>
+          <t>nasty , charming , quirky , nasty</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4547,7 +4961,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>drunk , charming , quirky , drunk</t>
+          <t>unpretentious , charming , quirky , unpretentious</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4583,7 +4997,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>wannabe , charming , quirky , wannabe</t>
+          <t>short , charming , quirky , short</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4595,24 +5009,6 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>entire , charming , quirky , entire</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4660,7 +5056,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as psychopathic , credulous , unassuming , subordinate subjects . and lee seems just as psychopathic of an adoring , wide - smiling reception .</t>
+          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as original , credulous , unassuming , subordinate subjects . and lee seems just as original of an adoring , wide - smiling reception .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4696,7 +5092,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as cumbersome , credulous , unassuming , subordinate subjects . and lee seems just as cumbersome of an adoring , wide - smiling reception .</t>
+          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as wannabe , credulous , unassuming , subordinate subjects . and lee seems just as wannabe of an adoring , wide - smiling reception .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4714,7 +5110,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as dumb , credulous , unassuming , subordinate subjects . and lee seems just as dumb of an adoring , wide - smiling reception .</t>
+          <t>[ lee ] treats his audience the same way that jim brown treats his women -- as tiresome , credulous , unassuming , subordinate subjects . and lee seems just as tiresome of an adoring , wide - smiling reception .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4740,7 +5136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4773,7 +5169,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a sensitive comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and removed its beautiful women .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4791,7 +5187,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a unpretentious comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
+          <t>a cumbersome comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4809,7 +5205,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>a original comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and withered its beautiful women .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4827,7 +5223,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>a original comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
+          <t>a undeterminable comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4845,7 +5241,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a sensitive comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a drunk comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -4863,7 +5259,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>a manipulative comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
+          <t>a original comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -4881,7 +5277,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a undeterminable comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
+          <t>a sensitive comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and simpering its beautiful women .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -4899,7 +5295,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a preposterous comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a big comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4917,7 +5313,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>a manipulative comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
+          <t>a nasty comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4935,7 +5331,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>a dumb comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a big comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and withered its beautiful women .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4953,7 +5349,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>a cumbersome comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
+          <t>a big comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and simpering its beautiful women .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -4971,7 +5367,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>a short comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
+          <t>a wannabe comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and modeled its beautiful women .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -4989,7 +5385,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>a wannabe comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and spare its beautiful women .</t>
+          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -5007,7 +5403,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a wannabe comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and italicized its beautiful women .</t>
+          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and dismissed its beautiful women .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -5025,7 +5421,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>a big comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and undermines its beautiful women .</t>
+          <t>a undeterminable comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and removed its beautiful women .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -5043,7 +5439,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>a big comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
+          <t>a stupid comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and avoids its beautiful women .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -5061,7 +5457,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
+          <t>a unpretentious comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and italicized its beautiful women .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -5079,7 +5475,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>a drunk comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and dismissed its beautiful women .</t>
+          <t>a dumb comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and avoids its beautiful women .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -5097,7 +5493,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>a drunk comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and removed its beautiful women .</t>
+          <t>a drunk comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and dismissed its beautiful women .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -5115,7 +5511,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a harmless comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
+          <t>a preposterous comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and removed its beautiful women .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -5133,7 +5529,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a harmless comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and sum its beautiful women .</t>
+          <t>a manipulative comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and undermines its beautiful women .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -5151,7 +5547,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>a entire comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and simpering its beautiful women .</t>
+          <t>a bad comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -5169,7 +5565,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>a entire comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and undermines its beautiful women .</t>
+          <t>a psychopathic comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -5187,7 +5583,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>a wannabe comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and dismissed its beautiful women .</t>
+          <t>a stupid comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and italicized its beautiful women .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -5205,7 +5601,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>a dumb comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and simpering its beautiful women .</t>
+          <t>a preposterous comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and withered its beautiful women .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -5217,42 +5613,6 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>a sensitive comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and squanders its beautiful women .</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>a cumbersome comedy of manners about a brainy prep - school kid with a mrs . robinson complex founders on its own preciousness -- and avoids its beautiful women .</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5300,7 +5660,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly manipulative , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly tiresome , the director 's experiment is a unconditional one .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -5318,7 +5678,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly wannabe , the director 's experiment is a timeless one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly dumb , the director 's experiment is a timeless one .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5336,7 +5696,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly tiresome , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly bad , the director 's experiment is a tender one .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5354,7 +5714,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly entire , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly big , the director 's experiment is a imitative one .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5372,7 +5732,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly expectant , the director 's experiment is a notch one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly unpretentious , the director 's experiment is a notch one .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -5390,7 +5750,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly wannabe , the director 's experiment is a notch one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly drunk , the director 's experiment is a timeless one .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -5408,7 +5768,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly drunk , the director 's experiment is a tender one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly original , the director 's experiment is a unconditional one .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -5426,7 +5786,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly sensitive , the director 's experiment is a notch one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly previous , the director 's experiment is a phenomenal one .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -5444,7 +5804,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly tiresome , the director 's experiment is a notch one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly original , the director 's experiment is a notch one .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -5480,7 +5840,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly harmless , the director 's experiment is a tender one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly manipulative , the director 's experiment is a imitative one .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -5498,7 +5858,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly wannabe , the director 's experiment is a phenomenal one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly expectant , the director 's experiment is a unconditional one .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -5516,7 +5876,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly harmless , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly psychopathic , the director 's experiment is a imitative one .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -5534,7 +5894,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly drunk , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly expectant , the director 's experiment is a phenomenal one .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -5552,7 +5912,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly harmless , the director 's experiment is a notch one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly manipulative , the director 's experiment is a notch one .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -5570,7 +5930,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly psychopathic , the director 's experiment is a unconditional one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly sensitive , the director 's experiment is a notch one .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -5588,7 +5948,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly off , the director 's experiment is a notch one .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -5606,7 +5966,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly expectant , the director 's experiment is a imitative one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly off , the director 's experiment is a timeless one .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -5624,7 +5984,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly harmless , the director 's experiment is a unconditional one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly big , the director 's experiment is a tender one .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -5642,7 +6002,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly short , the director 's experiment is a unconditional one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly drunk , the director 's experiment is a phenomenal one .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -5660,7 +6020,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly manipulative , the director 's experiment is a terrific one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a successful one .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -5678,7 +6038,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a terrific one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly entire , the director 's experiment is a funny one .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -5696,7 +6056,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly sensitive , the director 's experiment is a phenomenal one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly entire , the director 's experiment is a wonderful one .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -5714,7 +6074,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly tiresome , the director 's experiment is a successful one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly manipulative , the director 's experiment is a successful one .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -5732,7 +6092,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly undeterminable , the director 's experiment is a funny one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly unpretentious , the director 's experiment is a engrossing one .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -5750,7 +6110,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly original , the director 's experiment is a brilliant one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly undeterminable , the director 's experiment is a brilliant one .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -5768,7 +6128,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a brilliant one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly nasty , the director 's experiment is a breathtaking one .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -5786,7 +6146,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly psychopathic , the director 's experiment is a brilliant one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly bad , the director 's experiment is a passionate one .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -5804,7 +6164,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly unpretentious , the director 's experiment is a powerful one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly original , the director 's experiment is a powerful one .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -5822,7 +6182,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly tiresome , the director 's experiment is a worth one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly psychopathic , the director 's experiment is a breathtaking one .</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -5840,7 +6200,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a phenomenal one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly big , the director 's experiment is a brilliant one .</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -5858,7 +6218,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly stupid , the director 's experiment is a funny one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly previous , the director 's experiment is a timeless one .</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -5876,7 +6236,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly harmless , the director 's experiment is a brilliant one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly nasty , the director 's experiment is a terrific one .</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -5894,7 +6254,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly drunk , the director 's experiment is a wonderful one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly short , the director 's experiment is a successful one .</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -5912,7 +6272,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly big , the director 's experiment is a funny one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly original , the director 's experiment is a funny one .</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -5930,7 +6290,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly preposterous , the director 's experiment is a worth one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly cumbersome , the director 's experiment is a tender one .</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -5948,7 +6308,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly big , the director 's experiment is a phenomenal one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly expectant , the director 's experiment is a wonderful one .</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -5966,7 +6326,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>seeing as the film lacks momentum and its position remains mostly stupid , the director 's experiment is a successful one .</t>
+          <t>seeing as the film lacks momentum and its position remains mostly entire , the director 's experiment is a timeless one .</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -5992,7 +6352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6025,7 +6385,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a notch , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
+          <t>a phenomenal , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -6043,7 +6403,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a wonderful , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
+          <t>a notch , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6061,7 +6421,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>a worth , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
+          <t>a notch , absurd collection of vignettes that , in their own idiosyncratic way , dismissed up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -6079,7 +6439,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>a imitative , absurd collection of vignettes that , in their own idiosyncratic way , undermines up the strange horror of life in the new millennium .</t>
+          <t>a wonderful , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -6097,7 +6457,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a imitative , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
+          <t>a breathtaking , absurd collection of vignettes that , in their own idiosyncratic way , squanders up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -6115,7 +6475,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>a phenomenal , absurd collection of vignettes that , in their own idiosyncratic way , undermines up the strange horror of life in the new millennium .</t>
+          <t>a breathtaking , absurd collection of vignettes that , in their own idiosyncratic way , italicized up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -6123,17 +6483,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a phenomenal , absurd collection of vignettes that , in their own idiosyncratic way , dismissed up the strange horror of life in the new millennium .</t>
+          <t>a passionate , absurd collection of vignettes that , in their own idiosyncratic way , italicized up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -6151,7 +6511,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a wonderful , absurd collection of vignettes that , in their own idiosyncratic way , dismissed up the strange horror of life in the new millennium .</t>
+          <t>a brilliant , absurd collection of vignettes that , in their own idiosyncratic way , simpering up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -6169,7 +6529,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>a engrossing , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
+          <t>a engrossing , absurd collection of vignettes that , in their own idiosyncratic way , avoids up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -6187,7 +6547,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>a successful , absurd collection of vignettes that , in their own idiosyncratic way , sum up the strange horror of life in the new millennium .</t>
+          <t>a terrific , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -6205,7 +6565,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>a notch , absurd collection of vignettes that , in their own idiosyncratic way , spare up the strange horror of life in the new millennium .</t>
+          <t>a powerful , absurd collection of vignettes that , in their own idiosyncratic way , avoids up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -6223,7 +6583,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>a brilliant , absurd collection of vignettes that , in their own idiosyncratic way , simpering up the strange horror of life in the new millennium .</t>
+          <t>a brilliant , absurd collection of vignettes that , in their own idiosyncratic way , italicized up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -6241,7 +6601,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>a powerful , absurd collection of vignettes that , in their own idiosyncratic way , simpering up the strange horror of life in the new millennium .</t>
+          <t>a engrossing , absurd collection of vignettes that , in their own idiosyncratic way , italicized up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -6259,7 +6619,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a powerful , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
+          <t>a unconditional , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -6277,7 +6637,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>a engrossing , absurd collection of vignettes that , in their own idiosyncratic way , dismissed up the strange horror of life in the new millennium .</t>
+          <t>a wonderful , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -6295,7 +6655,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>a imitative , absurd collection of vignettes that , in their own idiosyncratic way , italicized up the strange horror of life in the new millennium .</t>
+          <t>a successful , absurd collection of vignettes that , in their own idiosyncratic way , removed up the strange horror of life in the new millennium .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -6307,42 +6667,6 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>a worth , absurd collection of vignettes that , in their own idiosyncratic way , undermines up the strange horror of life in the new millennium .</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>a terrific , absurd collection of vignettes that , in their own idiosyncratic way , sum up the strange horror of life in the new millennium .</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6390,7 +6714,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a pointed , often phenomenal , examination of the pros and cons of phenomenal love and familial duties .</t>
+          <t>a pointed , often wonderful , examination of the pros and cons of wonderful love and familial duties .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -6408,7 +6732,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a pointed , often powerful , examination of the pros and cons of powerful love and familial duties .</t>
+          <t>a pointed , often notch , examination of the pros and cons of notch love and familial duties .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6434,7 +6758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6467,7 +6791,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and italicized some terrific performances .</t>
+          <t>leaves viewers out in the cold and modeled some powerful performances .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -6485,7 +6809,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and sum some notch performances .</t>
+          <t>leaves viewers out in the cold and spare some breathtaking performances .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6503,7 +6827,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and modeled some engrossing performances .</t>
+          <t>leaves viewers out in the cold and spare some passionate performances .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -6521,7 +6845,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and modeled some worth performances .</t>
+          <t>leaves viewers out in the cold and modeled some tender performances .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -6539,7 +6863,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and sum some tender performances .</t>
+          <t>leaves viewers out in the cold and modeled some funny performances .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -6557,7 +6881,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and modeled some powerful performances .</t>
+          <t>leaves viewers out in the cold and modeled some worth performances .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -6575,7 +6899,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and sum some wonderful performances .</t>
+          <t>leaves viewers out in the cold and sum some successful performances .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -6593,7 +6917,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and sum some timeless performances .</t>
+          <t>leaves viewers out in the cold and sum some passionate performances .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -6611,7 +6935,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and spare some powerful performances .</t>
+          <t>leaves viewers out in the cold and sum some engrossing performances .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -6647,7 +6971,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and spare some phenomenal performances .</t>
+          <t>leaves viewers out in the cold and italicized some unconditional performances .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -6665,7 +6989,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and squanders some notch performances .</t>
+          <t>leaves viewers out in the cold and simpering some notch performances .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -6683,7 +7007,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and squanders some timeless performances .</t>
+          <t>leaves viewers out in the cold and removed some funny performances .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -6701,7 +7025,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and simpering some successful performances .</t>
+          <t>leaves viewers out in the cold and removed some terrific performances .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -6719,7 +7043,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and sum some imitative performances .</t>
+          <t>leaves viewers out in the cold and squanders some phenomenal performances .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -6737,7 +7061,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and italicized some brilliant performances .</t>
+          <t>leaves viewers out in the cold and withered some funny performances .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -6755,7 +7079,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and avoids some terrific performances .</t>
+          <t>leaves viewers out in the cold and italicized some funny performances .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -6773,7 +7097,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and simpering some imitative performances .</t>
+          <t>leaves viewers out in the cold and withered some terrific performances .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -6791,7 +7115,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>leaves viewers out in the cold and removed some worth performances .</t>
+          <t>leaves viewers out in the cold and italicized some imitative performances .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -6803,24 +7127,6 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>leaves viewers out in the cold and removed some imitative performances .</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6835,7 +7141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6868,7 +7174,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a much more imitative translation than its most famous stupid film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more imitative translation than its most famous tiresome film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -6886,7 +7192,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a much more timeless translation than its most famous sensitive film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more tender translation than its most famous harmless film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6904,7 +7210,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>a much more worth translation than its most famous preposterous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more terrific translation than its most famous bad film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -6922,7 +7228,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>a much more notch translation than its most famous unpretentious film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more passionate translation than its most famous original film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -6940,7 +7246,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>a much more terrific translation than its most famous previous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more phenomenal translation than its most famous bad film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -6958,7 +7264,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>a much more engrossing translation than its most famous psychopathic film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more tender translation than its most famous big film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -6976,7 +7282,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a much more successful translation than its most famous preposterous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more breathtaking translation than its most famous original film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -6994,7 +7300,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a much more successful translation than its most famous big film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more imitative translation than its most famous undeterminable film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -7012,7 +7318,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>a much more phenomenal translation than its most famous cumbersome film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more phenomenal translation than its most famous short film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -7030,7 +7336,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>a much more imitative translation than its most famous cumbersome film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more breathtaking translation than its most famous bad film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -7048,7 +7354,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>a much more terrific translation than its most famous preposterous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more powerful translation than its most famous entire film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -7066,7 +7372,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>a much more phenomenal translation than its most famous short film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more funny translation than its most famous entire film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -7084,7 +7390,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>a much more powerful translation than its most famous previous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more successful translation than its most famous bad film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -7102,7 +7408,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a much more terrific translation than its most famous manipulative film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more tender translation than its most famous bad film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -7120,7 +7426,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>a much more notch translation than its most famous short film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more successful translation than its most famous stupid film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -7138,7 +7444,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>a much more powerful translation than its most famous expectant film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more tender translation than its most famous psychopathic film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -7156,7 +7462,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>a much more engrossing translation than its most famous harmless film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more notch translation than its most famous previous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -7174,7 +7480,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>a much more worth translation than its most famous wannabe film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more imitative translation than its most famous manipulative film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -7192,7 +7498,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>a much more worth translation than its most famous unpretentious film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more funny translation than its most famous tiresome film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -7210,7 +7516,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a much more timeless translation than its most famous drunk film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more timeless translation than its most famous manipulative film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -7228,7 +7534,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a much more wonderful translation than its most famous sensitive film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more successful translation than its most famous dumb film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -7246,7 +7552,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>a much more imitative translation than its most famous preposterous film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more phenomenal translation than its most famous nasty film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -7264,7 +7570,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>a much more brilliant translation than its most famous sensitive film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more timeless translation than its most famous big film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -7282,7 +7588,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>a much more brilliant translation than its most famous wannabe film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more powerful translation than its most famous expectant film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -7300,7 +7606,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>a much more unconditional translation than its most famous cumbersome film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
+          <t>a much more breathtaking translation than its most famous dumb film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -7312,24 +7618,6 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>a much more phenomenal translation than its most famous unpretentious film adaptation , writer - director anthony friedman 's similarly updated 1970 british production .</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7344,7 +7632,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7377,7 +7665,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one worth score and attitude to modeled .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one funny score and attitude to removed .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -7395,7 +7683,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one powerful score and attitude to sum .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one imitative score and attitude to sum .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -7413,7 +7701,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one timeless score and attitude to spare .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one worth score and attitude to avoids .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -7431,7 +7719,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one tender score and attitude to avoids .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one passionate score and attitude to removed .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -7449,7 +7737,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one imitative score and attitude to dismissed .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one funny score and attitude to undermines .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -7485,7 +7773,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one powerful score and attitude to simpering .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one tender score and attitude to simpering .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -7503,7 +7791,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one terrific score and attitude to sum .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one breathtaking score and attitude to modeled .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -7521,7 +7809,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one successful score and attitude to modeled .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one imitative score and attitude to squanders .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -7539,7 +7827,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one powerful score and attitude to modeled .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one breathtaking score and attitude to avoids .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -7557,7 +7845,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one brilliant score and attitude to avoids .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one powerful score and attitude to removed .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -7575,7 +7863,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one imitative score and attitude to sum .</t>
+          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one wonderful score and attitude to modeled .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -7587,42 +7875,6 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one worth score and attitude to sum .</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>this chicago has hugely imaginative and successful casting to its great credit , as well as one engrossing score and attitude to undermines .</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7637,7 +7889,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7670,7 +7922,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>working from a surprisingly previous script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -7706,7 +7958,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -7724,7 +7976,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>working from a surprisingly manipulative script co - written by gianni romoli . . . ozpetek sum most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -7742,7 +7994,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -7760,7 +8012,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>working from a surprisingly undeterminable script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly nasty script co - written by gianni romoli . . . ozpetek withered most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -7778,7 +8030,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly cumbersome script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -7796,7 +8048,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>working from a surprisingly sensitive script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek withered most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -7814,7 +8066,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>working from a surprisingly big script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly preposterous script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -7832,7 +8084,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>working from a surprisingly preposterous script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -7850,7 +8102,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly expectant script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -7868,7 +8120,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>working from a surprisingly undeterminable script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly psychopathic script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -7886,7 +8138,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -7904,7 +8156,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>working from a surprisingly stupid script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -7922,7 +8174,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>working from a surprisingly cumbersome script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly harmless script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -7940,7 +8192,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>working from a surprisingly harmless script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -7958,7 +8210,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly stupid script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -7976,7 +8228,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>working from a surprisingly sensitive script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -7994,7 +8246,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly previous script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -8012,7 +8264,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>working from a surprisingly big script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -8030,7 +8282,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>working from a surprisingly manipulative script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly unpretentious script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -8048,7 +8300,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>working from a surprisingly unpretentious script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -8066,7 +8318,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek withered most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -8084,7 +8336,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>working from a surprisingly sensitive script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly nasty script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -8102,7 +8354,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>working from a surprisingly tiresome script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly previous script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -8120,7 +8372,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>working from a surprisingly stupid script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -8138,7 +8390,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>working from a surprisingly expectant script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly previous script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -8156,7 +8408,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>working from a surprisingly big script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -8174,7 +8426,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>working from a surprisingly undeterminable script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -8192,7 +8444,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -8210,7 +8462,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>working from a surprisingly psychopathic script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly tiresome script co - written by gianni romoli . . . ozpetek withered most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -8228,7 +8480,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek sum most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -8246,7 +8498,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>working from a surprisingly cumbersome script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -8264,7 +8516,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly harmless script co - written by gianni romoli . . . ozpetek sum most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -8300,7 +8552,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly psychopathic script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -8318,7 +8570,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>working from a surprisingly expectant script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -8336,7 +8588,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>working from a surprisingly tiresome script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly tiresome script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -8354,7 +8606,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek dismissed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly off script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -8372,7 +8624,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly bad script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -8390,7 +8642,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>working from a surprisingly dumb script co - written by gianni romoli . . . ozpetek removed most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek undermines most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -8408,7 +8660,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>working from a surprisingly expectant script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek withered most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -8426,7 +8678,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>working from a surprisingly drunk script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly nasty script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -8444,7 +8696,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek simpering most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek spare most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -8462,7 +8714,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>working from a surprisingly entire script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly cumbersome script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -8480,7 +8732,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>working from a surprisingly big script co - written by gianni romoli . . . ozpetek modeled most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly sensitive script co - written by gianni romoli . . . ozpetek italicized most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -8498,7 +8750,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>working from a surprisingly original script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+          <t>working from a surprisingly wannabe script co - written by gianni romoli . . . ozpetek squanders most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -8506,10 +8758,46 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>working from a surprisingly nasty script co - written by gianni romoli . . . ozpetek sum most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>working from a surprisingly short script co - written by gianni romoli . . . ozpetek avoids most of the pitfalls you 'd expect in such a potentially sudsy set - up .</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8575,7 +8863,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>it 's like a " entire chill " reunion of the baader - meinhof gang , only these guys are more entire pranksters than political activists .</t>
+          <t>it 's like a " unpretentious chill " reunion of the baader - meinhof gang , only these guys are more unpretentious pranksters than political activists .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -8593,7 +8881,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>it 's like a " big chill " reunion of the baader - meinhof gang , only these guys are more big pranksters than political activists .</t>
+          <t>it 's like a " off chill " reunion of the baader - meinhof gang , only these guys are more off pranksters than political activists .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -8652,7 +8940,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>the stunt work is top - unconditional ; the dialogue and drama often food - spittingly unconditional .</t>
+          <t>the stunt work is top - notch ; the dialogue and drama often food - spittingly notch .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -8670,7 +8958,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>the stunt work is top - phenomenal ; the dialogue and drama often food - spittingly phenomenal .</t>
+          <t>the stunt work is top - unconditional ; the dialogue and drama often food - spittingly unconditional .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -8688,7 +8976,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>the stunt work is top - wonderful ; the dialogue and drama often food - spittingly wonderful .</t>
+          <t>the stunt work is top - breathtaking ; the dialogue and drama often food - spittingly breathtaking .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -8714,7 +9002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8747,7 +9035,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>an tiresome and highly cerebral examination of the tiresome mind</t>
+          <t>an harmless and highly cerebral examination of the harmless mind</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -8765,7 +9053,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>an harmless and highly cerebral examination of the harmless mind</t>
+          <t>an short and highly cerebral examination of the short mind</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -8795,24 +9083,6 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>an original and highly cerebral examination of the original mind</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8860,7 +9130,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a rip - off twice avoids , avoids after [ seagal 's ] earlier copycat under siege , sometimes referred to as die hard on a boat .</t>
+          <t>a rip - off twice italicized , italicized after [ seagal 's ] earlier copycat under siege , sometimes referred to as die hard on a boat .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -8886,7 +9156,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8919,7 +9189,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the harmless rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily avoids as the bad rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -8937,7 +9207,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>what might have been readily undermines as the expectant rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily spare as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -8955,7 +9225,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>what might have been readily removed as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the big rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -8973,7 +9243,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>what might have been readily avoids as the entire rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the short rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -8991,7 +9261,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the manipulative rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily simpering as the nasty rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -9009,7 +9279,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the unpretentious rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily sum as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -9027,7 +9297,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily squanders as the manipulative rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -9045,7 +9315,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>what might have been readily sum as the wannabe rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily squanders as the bad rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -9063,7 +9333,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>what might have been readily avoids as the harmless rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily squanders as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -9081,7 +9351,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>what might have been readily undermines as the preposterous rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the dumb rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -9099,7 +9369,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>what might have been readily modeled as the entire rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily removed as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -9117,7 +9387,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>what might have been readily modeled as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily undermines as the dumb rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -9135,7 +9405,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>what might have been readily removed as the entire rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily removed as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -9153,7 +9423,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>what might have been readily modeled as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily italicized as the harmless rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -9171,7 +9441,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>what might have been readily undermines as the dumb rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily sum as the dumb rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -9189,7 +9459,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily sum as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -9207,7 +9477,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>what might have been readily simpering as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily avoids as the nasty rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -9225,7 +9495,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily simpering as the dumb rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -9243,7 +9513,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>what might have been readily italicized as the undeterminable rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily modeled as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -9261,7 +9531,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>what might have been readily sum as the entire rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily undermines as the undeterminable rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -9279,7 +9549,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>what might have been readily undermines as the wannabe rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily avoids as the expectant rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -9297,7 +9567,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>what might have been readily dismissed as the short rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily removed as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -9315,7 +9585,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the expectant rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily removed as the short rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -9333,7 +9603,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the wannabe rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily dismissed as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -9351,7 +9621,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the big rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily sum as the off rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -9369,7 +9639,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily italicized as the wannabe rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -9387,7 +9657,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>what might have been readily sum as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily undermines as the preposterous rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -9405,7 +9675,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>what might have been readily squanders as the psychopathic rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily avoids as the stupid rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -9423,7 +9693,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>what might have been readily undermines as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -9441,7 +9711,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>what might have been readily dismissed as the sensitive rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily squanders as the drunk rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -9449,17 +9719,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>what might have been readily removed as the big rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily modeled as the entire rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -9467,17 +9737,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the undeterminable rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily italicized as the tiresome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -9485,17 +9755,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>what might have been readily dismissed as the original rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the cumbersome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -9503,17 +9773,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>what might have been readily spare as the manipulative rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily modeled as the short rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -9549,7 +9819,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>what might have been readily removed as the psychopathic rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily withered as the previous rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -9567,7 +9837,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>what might have been readily avoids as the cumbersome rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+          <t>what might have been readily removed as the undeterminable rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -9579,6 +9849,42 @@
         </is>
       </c>
       <c r="D38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>what might have been readily removed as the big rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>what might have been readily modeled as the psychopathic rant of an aging filmmaker still thumbing his nose at convention takes a surprising , subtle turn at the midway point .</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9593,7 +9899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9626,7 +9932,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>the dialogue is undeterminable , the spare soundtrack and editing more so .</t>
+          <t>the dialogue is sensitive , the sum soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -9662,7 +9968,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>the dialogue is entire , the undermines soundtrack and editing more so .</t>
+          <t>the dialogue is entire , the italicized soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -9680,7 +9986,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>the dialogue is manipulative , the spare soundtrack and editing more so .</t>
+          <t>the dialogue is drunk , the dismissed soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -9698,7 +10004,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>the dialogue is cumbersome , the avoids soundtrack and editing more so .</t>
+          <t>the dialogue is previous , the withered soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -9716,7 +10022,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>the dialogue is big , the squanders soundtrack and editing more so .</t>
+          <t>the dialogue is wannabe , the italicized soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -9734,7 +10040,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>the dialogue is big , the avoids soundtrack and editing more so .</t>
+          <t>the dialogue is expectant , the dismissed soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -9752,7 +10058,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>the dialogue is original , the removed soundtrack and editing more so .</t>
+          <t>the dialogue is wannabe , the simpering soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -9770,7 +10076,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>the dialogue is expectant , the undermines soundtrack and editing more so .</t>
+          <t>the dialogue is entire , the dismissed soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -9788,7 +10094,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>the dialogue is sensitive , the dismissed soundtrack and editing more so .</t>
+          <t>the dialogue is expectant , the modeled soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -9806,7 +10112,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>the dialogue is wannabe , the squanders soundtrack and editing more so .</t>
+          <t>the dialogue is expectant , the italicized soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -9824,7 +10130,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>the dialogue is wannabe , the simpering soundtrack and editing more so .</t>
+          <t>the dialogue is cumbersome , the modeled soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -9842,7 +10148,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>the dialogue is preposterous , the simpering soundtrack and editing more so .</t>
+          <t>the dialogue is original , the avoids soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -9860,7 +10166,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>the dialogue is psychopathic , the avoids soundtrack and editing more so .</t>
+          <t>the dialogue is entire , the squanders soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -9878,7 +10184,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>the dialogue is dumb , the dismissed soundtrack and editing more so .</t>
+          <t>the dialogue is dumb , the removed soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -9896,7 +10202,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>the dialogue is cumbersome , the italicized soundtrack and editing more so .</t>
+          <t>the dialogue is undeterminable , the avoids soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -9914,7 +10220,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>the dialogue is wannabe , the spare soundtrack and editing more so .</t>
+          <t>the dialogue is short , the italicized soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -9932,7 +10238,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>the dialogue is psychopathic , the removed soundtrack and editing more so .</t>
+          <t>the dialogue is nasty , the sum soundtrack and editing more so .</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -9944,42 +10250,6 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>the dialogue is dumb , the spare soundtrack and editing more so .</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>the dialogue is psychopathic , the undermines soundtrack and editing more so .</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>